<commit_message>
Add ManageView and UserView, modify UploadExcel for parsing Excels of 4 sheets
</commit_message>
<xml_diff>
--- a/clusters/tests/test_models/excel_test_file/cl_example.xlsx
+++ b/clusters/tests/test_models/excel_test_file/cl_example.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E022B6EC-D9D7-4AE7-932F-267BAA0C9C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xpeppers/Desktop/career-landscape/clusters/tests/test_models/excel_test_file/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D277BC52-AE9A-0F47-B6F9-7D77A01BDDE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="660" windowWidth="21940" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>User Information</t>
   </si>
@@ -73,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +178,32 @@
     <tableColumn id="3" xr3:uid="{76DBF87F-133C-4549-B4FF-F2BF9DD376FD}" name="Nome"/>
     <tableColumn id="4" xr3:uid="{8B999421-C6E6-401A-AB2F-C235DE1ED372}" name="Cognome"/>
     <tableColumn id="5" xr3:uid="{BCD39146-C78F-4B6C-8254-5DF4CE8B68FC}" name="data"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{660C5CE8-24F3-9D46-9316-D5BF23AFBD43}" name="Table23" displayName="Table23" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{E12D16BE-25C9-8C42-B6EE-E22C757BFF56}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CB8F2CEE-34B6-D14C-87F2-E4C932371180}" name="User Information"/>
+    <tableColumn id="3" xr3:uid="{000F7078-C146-E848-9076-C77E52F825D2}" name="Nome"/>
+    <tableColumn id="4" xr3:uid="{AA533DEE-041C-EC41-9D4E-590CFBFAEE98}" name="Cognome"/>
+    <tableColumn id="5" xr3:uid="{2D13B7A6-6EA1-DD4D-8EC1-7B0859F129BE}" name="data"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2008E05-5488-B042-9C41-5A6F25FF3045}" name="Table24" displayName="Table24" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{FE73B143-B6B4-6B4A-9636-1864449E6886}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3CDCFB23-7586-DF47-8D68-F3F7010149E5}" name="User Information"/>
+    <tableColumn id="3" xr3:uid="{E1D16338-565B-D347-8987-1299A853B6D9}" name="Nome"/>
+    <tableColumn id="4" xr3:uid="{09FD26A4-C866-B543-9A72-979D6A243727}" name="Cognome"/>
+    <tableColumn id="5" xr3:uid="{5958167C-022A-6441-B6B9-9DC5116A947C}" name="data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -475,12 +509,12 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -505,17 +539,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -523,7 +557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -534,7 +568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -545,7 +579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -556,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -567,10 +601,226 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C4799C-8486-2945-B264-DD755FF1F5DA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A4F75-9F43-9C40-B93F-89CDDDAFE57C}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE70F21-8573-EA43-84BB-E83EC5572B18}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>